<commit_message>
almost finish transport order flow
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -59,6 +59,51 @@
   </si>
   <si>
     <t>NUMBER_OF_CART</t>
+  </si>
+  <si>
+    <t>GOODS_LONGER_THAN_6_FT</t>
+  </si>
+  <si>
+    <t>GOODS_TALLER_THAN_2_FT</t>
+  </si>
+  <si>
+    <t>PET_FRIENDLY</t>
+  </si>
+  <si>
+    <t>ENGLISH_SPEAKING</t>
+  </si>
+  <si>
+    <t>TUNNEL_PREFERENCE</t>
+  </si>
+  <si>
+    <t>SELECTED_TUNNEL</t>
+  </si>
+  <si>
+    <t>MOVE_DOOR_TO_DOOR</t>
+  </si>
+  <si>
+    <t>TRANSPORT_OR_DISPOSE_WASTE</t>
+  </si>
+  <si>
+    <t>USER_NAME</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER</t>
+  </si>
+  <si>
+    <t>EXTENSION_FLAG</t>
+  </si>
+  <si>
+    <t>EXTENSION</t>
+  </si>
+  <si>
+    <t>TIP</t>
+  </si>
+  <si>
+    <t>COUPON</t>
+  </si>
+  <si>
+    <t>PAYMENT_METHOD</t>
   </si>
   <si>
     <t>TC001_Complete a transport order with testing account</t>
@@ -95,7 +140,7 @@
     <t>Today</t>
   </si>
   <si>
-    <t>01 Aug</t>
+    <t>Tomorrow</t>
   </si>
   <si>
     <t>ASAP</t>
@@ -104,7 +149,7 @@
     <t>No hourly rental</t>
   </si>
   <si>
-    <t>Premium Van</t>
+    <t>Van</t>
   </si>
   <si>
     <t>Basic</t>
@@ -114,6 +159,30 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>Tai Lam Tunnel</t>
+  </si>
+  <si>
+    <t>William Koh</t>
+  </si>
+  <si>
+    <t>51112222</t>
+  </si>
+  <si>
+    <t>852</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>FPS</t>
   </si>
 </sst>
 </file>
@@ -1328,14 +1397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16" width="16.3516" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="31" width="16.3516" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
@@ -1387,22 +1456,67 @@
       <c r="P1" t="s" s="2">
         <v>15</v>
       </c>
+      <c r="Q1" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" ht="22.55" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5">
         <v>12345678</v>
       </c>
       <c r="D2" t="s" s="6">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s" s="6">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F2" t="b" s="7">
         <v>0</v>
@@ -1411,31 +1525,76 @@
         <v>0</v>
       </c>
       <c r="H2" t="s" s="6">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s" s="6">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s" s="6">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s" s="6">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s" s="6">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s" s="6">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="N2" t="s" s="6">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="O2" t="s" s="6">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s" s="6">
-        <v>28</v>
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="R2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="S2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="U2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="V2" t="s" s="6">
+        <v>45</v>
+      </c>
+      <c r="W2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="Y2" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="Z2" t="s" s="6">
+        <v>47</v>
+      </c>
+      <c r="AA2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="AB2" t="s" s="6">
+        <v>48</v>
+      </c>
+      <c r="AC2" t="s" s="6">
+        <v>49</v>
+      </c>
+      <c r="AD2" t="s" s="6">
+        <v>50</v>
+      </c>
+      <c r="AE2" t="s" s="6">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update transport order for personal ac
update for end-to-end testing of personal account
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>PAYMENT_METHOD</t>
+  </si>
+  <si>
+    <t>CANCEL_FLAG</t>
+  </si>
+  <si>
+    <t>DRIVER_PHONE_NUMBER</t>
+  </si>
+  <si>
+    <t>DRIVER_PASSWORD</t>
   </si>
   <si>
     <t>TC001_Complete a transport order with testing account</t>
@@ -140,9 +149,6 @@
     <t>Today</t>
   </si>
   <si>
-    <t>Tomorrow</t>
-  </si>
-  <si>
     <t>ASAP</t>
   </si>
   <si>
@@ -161,7 +167,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>TRUE</t>
+    <t>FALSE</t>
   </si>
   <si>
     <t>Tai Lam Tunnel</t>
@@ -179,10 +185,16 @@
     <t>20</t>
   </si>
   <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>FPS</t>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>66778899</t>
+  </si>
+  <si>
+    <t>Qa12345!</t>
   </si>
 </sst>
 </file>
@@ -320,7 +332,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -344,6 +356,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1397,14 +1412,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="31" width="16.3516" style="1" customWidth="1"/>
-    <col min="32" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="34" width="16.3516" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
@@ -1501,22 +1516,31 @@
       <c r="AE1" t="s" s="2">
         <v>30</v>
       </c>
+      <c r="AF1" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s" s="2">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" ht="22.55" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" s="5">
         <v>12345678</v>
       </c>
       <c r="D2" t="s" s="6">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s" s="6">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F2" t="b" s="7">
         <v>0</v>
@@ -1525,76 +1549,85 @@
         <v>0</v>
       </c>
       <c r="H2" t="s" s="6">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s" s="6">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s" s="6">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K2" t="s" s="6">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L2" t="s" s="6">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M2" t="s" s="6">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s" s="6">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O2" t="s" s="6">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="P2" t="s" s="6">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Q2" t="s" s="6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R2" t="s" s="6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="S2" t="s" s="6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T2" t="s" s="6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="U2" t="s" s="6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V2" t="s" s="6">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="W2" t="s" s="6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="X2" t="s" s="6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Y2" t="s" s="6">
+        <v>48</v>
+      </c>
+      <c r="Z2" t="s" s="6">
+        <v>49</v>
+      </c>
+      <c r="AA2" t="s" s="6">
         <v>46</v>
       </c>
-      <c r="Z2" t="s" s="6">
-        <v>47</v>
-      </c>
-      <c r="AA2" t="s" s="6">
-        <v>44</v>
-      </c>
       <c r="AB2" t="s" s="6">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AC2" t="s" s="6">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AD2" t="s" s="6">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AE2" t="s" s="6">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="AF2" t="s" s="6">
+        <v>53</v>
+      </c>
+      <c r="AG2" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="AH2" t="s" s="6">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the Transport order automation
Added the business account automation process
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -11,11 +11,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>TEST_CASE</t>
   </si>
   <si>
+    <t>ACCOUNT_TYPE</t>
+  </si>
+  <si>
     <t>EMAIL_OR_PHONENUMBER</t>
   </si>
   <si>
@@ -115,7 +118,10 @@
     <t>DRIVER_PASSWORD</t>
   </si>
   <si>
-    <t>TC001_Complete a transport order with testing account</t>
+    <t>TC001_Complete a transport order with testing personal account</t>
+  </si>
+  <si>
+    <t>Personal</t>
   </si>
   <si>
     <r>
@@ -137,10 +143,10 @@
     </r>
   </si>
   <si>
-    <t>North point</t>
-  </si>
-  <si>
-    <t>Siu sai wan</t>
+    <t>Tin Hau</t>
+  </si>
+  <si>
+    <t>Tsim Sha Tsui</t>
   </si>
   <si>
     <t>Chai wan</t>
@@ -194,7 +200,43 @@
     <t>66778899</t>
   </si>
   <si>
-    <t>Qa12345!</t>
+    <t>Aa123456</t>
+  </si>
+  <si>
+    <t>TC002_Complete a transport order with testing business account</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>qadmaster1@gogotech.hk</t>
+  </si>
+  <si>
+    <t>Ma On Shan</t>
+  </si>
+  <si>
+    <t>Festival walk</t>
+  </si>
+  <si>
+    <t>Cityu</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Lion Rock Tunnel</t>
+  </si>
+  <si>
+    <t>QA Tester</t>
+  </si>
+  <si>
+    <t>No tip</t>
   </si>
 </sst>
 </file>
@@ -258,7 +300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -275,6 +317,51 @@
       </right>
       <top style="thin">
         <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -332,7 +419,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -358,6 +445,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1412,14 +1517,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="34" width="16.3516" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="35" width="16.3516" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
@@ -1525,114 +1630,227 @@
       <c r="AH1" t="s" s="2">
         <v>33</v>
       </c>
+      <c r="AI1" t="s" s="2">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" ht="22.55" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="C2" s="5">
+      <c r="B2" t="s" s="3">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="D2" s="5">
         <v>12345678</v>
       </c>
-      <c r="D2" t="s" s="6">
-        <v>36</v>
-      </c>
       <c r="E2" t="s" s="6">
-        <v>37</v>
-      </c>
-      <c r="F2" t="b" s="7">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="F2" t="s" s="6">
+        <v>39</v>
       </c>
       <c r="G2" t="b" s="7">
         <v>0</v>
       </c>
-      <c r="H2" t="s" s="6">
-        <v>38</v>
+      <c r="H2" t="b" s="7">
+        <v>0</v>
       </c>
       <c r="I2" t="s" s="6">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s" s="6">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K2" t="s" s="6">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L2" t="s" s="6">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M2" t="s" s="6">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N2" t="s" s="6">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O2" t="s" s="6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P2" t="s" s="6">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q2" t="s" s="6">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R2" t="s" s="6">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="S2" t="s" s="6">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="T2" t="s" s="6">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="U2" t="s" s="6">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="V2" t="s" s="6">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W2" t="s" s="6">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="X2" t="s" s="6">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Y2" t="s" s="6">
         <v>48</v>
       </c>
       <c r="Z2" t="s" s="6">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AA2" t="s" s="6">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="AB2" t="s" s="6">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AC2" t="s" s="6">
+        <v>52</v>
+      </c>
+      <c r="AD2" t="s" s="6">
+        <v>53</v>
+      </c>
+      <c r="AE2" t="s" s="6">
+        <v>48</v>
+      </c>
+      <c r="AF2" t="s" s="6">
+        <v>54</v>
+      </c>
+      <c r="AG2" t="s" s="6">
+        <v>55</v>
+      </c>
+      <c r="AH2" t="s" s="8">
+        <v>56</v>
+      </c>
+      <c r="AI2" t="s" s="6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" ht="22.55" customHeight="1">
+      <c r="A3" t="s" s="9">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s" s="9">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s" s="10">
+        <v>60</v>
+      </c>
+      <c r="D3" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="E3" t="s" s="12">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s" s="12">
+        <v>62</v>
+      </c>
+      <c r="G3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s" s="12">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s" s="12">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s" s="12">
+        <v>43</v>
+      </c>
+      <c r="N3" t="s" s="12">
+        <v>44</v>
+      </c>
+      <c r="O3" t="s" s="12">
+        <v>64</v>
+      </c>
+      <c r="P3" t="s" s="12">
+        <v>65</v>
+      </c>
+      <c r="Q3" t="s" s="12">
+        <v>66</v>
+      </c>
+      <c r="R3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="S3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="T3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="U3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="V3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="W3" t="s" s="12">
+        <v>67</v>
+      </c>
+      <c r="X3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="Y3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="Z3" t="s" s="12">
+        <v>68</v>
+      </c>
+      <c r="AA3" t="s" s="12">
         <v>51</v>
       </c>
-      <c r="AD2" t="s" s="6">
-        <v>46</v>
-      </c>
-      <c r="AE2" t="s" s="6">
+      <c r="AB3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="AC3" t="s" s="12">
         <v>52</v>
       </c>
-      <c r="AF2" t="s" s="6">
-        <v>53</v>
-      </c>
-      <c r="AG2" t="s" s="8">
+      <c r="AD3" t="s" s="12">
+        <v>69</v>
+      </c>
+      <c r="AE3" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="AF3" t="s" s="12">
         <v>54</v>
       </c>
-      <c r="AH2" t="s" s="6">
+      <c r="AG3" t="s" s="12">
         <v>55</v>
+      </c>
+      <c r="AH3" t="s" s="14">
+        <v>56</v>
+      </c>
+      <c r="AI3" t="s" s="12">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="" tooltip="" display="qa1@gogotech.hk "/>
+    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="qa1@gogotech.hk "/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
adding delivery order steps
added delivery order for pickup from and pickup to pages
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -112,13 +112,40 @@
     <t>CANCEL_FLAG</t>
   </si>
   <si>
+    <t>ORDER_TYPE</t>
+  </si>
+  <si>
+    <t>ESTATE_NUMBER_SENDER</t>
+  </si>
+  <si>
+    <t>ROOM_AND_FLOOR_SENDER</t>
+  </si>
+  <si>
+    <t>SENDER_NAME</t>
+  </si>
+  <si>
+    <t>SENDER_PHONE_NUMBER</t>
+  </si>
+  <si>
+    <t>ESTATE_NUMBER_RECIPIENT</t>
+  </si>
+  <si>
+    <t>ROOM_AND_FLOOR_RECIPIENT</t>
+  </si>
+  <si>
+    <t>RECIPIENT_NAME</t>
+  </si>
+  <si>
+    <t>RECIPIENT_PHONE_NUMBER</t>
+  </si>
+  <si>
     <t>DRIVER_PHONE_NUMBER</t>
   </si>
   <si>
     <t>DRIVER_PASSWORD</t>
   </si>
   <si>
-    <t>TC001_Complete a transport order with testing personal account</t>
+    <t>TC001_Complete a delivery order with testing personal account</t>
   </si>
   <si>
     <t>Personal</t>
@@ -197,13 +224,46 @@
     <t>False</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>North Point</t>
+  </si>
+  <si>
+    <t>3026A</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>92516783</t>
+  </si>
+  <si>
+    <t>Siu Sai Wan</t>
+  </si>
+  <si>
+    <t>4218B</t>
+  </si>
+  <si>
+    <t>William2</t>
+  </si>
+  <si>
+    <t>53326890</t>
+  </si>
+  <si>
     <t>66778899</t>
   </si>
   <si>
     <t>Aa123456</t>
   </si>
   <si>
-    <t>TC002_Complete a transport order with testing business account</t>
+    <t>TC002_Complete a transport order with testing personal account</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>TC003_Complete a transport order with testing business account</t>
   </si>
   <si>
     <t>Business</t>
@@ -300,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -364,7 +424,37 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
         <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -391,22 +481,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
         <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -419,7 +494,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -444,26 +519,32 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1517,14 +1598,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="35" width="16.3516" style="1" customWidth="1"/>
-    <col min="36" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="44" width="16.3516" style="1" customWidth="1"/>
+    <col min="45" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
@@ -1633,25 +1714,52 @@
       <c r="AI1" t="s" s="2">
         <v>34</v>
       </c>
+      <c r="AJ1" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s" s="2">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" ht="22.55" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5">
         <v>12345678</v>
       </c>
       <c r="E2" t="s" s="6">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s" s="6">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G2" t="b" s="7">
         <v>0</v>
@@ -1660,105 +1768,132 @@
         <v>0</v>
       </c>
       <c r="I2" t="s" s="6">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s" s="6">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="K2" t="s" s="6">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s" s="6">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="M2" t="s" s="6">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="N2" t="s" s="6">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O2" t="s" s="6">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="P2" t="s" s="6">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="Q2" t="s" s="6">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="R2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="S2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="T2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="U2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="V2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="W2" t="s" s="6">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="X2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="Y2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="Z2" t="s" s="6">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="AA2" t="s" s="6">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="AB2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AC2" t="s" s="6">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="AD2" t="s" s="6">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="AE2" t="s" s="6">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AF2" t="s" s="6">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="AG2" t="s" s="6">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="AH2" t="s" s="8">
-        <v>56</v>
-      </c>
-      <c r="AI2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="AI2" t="s" s="8">
+        <v>66</v>
+      </c>
+      <c r="AJ2" t="s" s="8">
+        <v>67</v>
+      </c>
+      <c r="AK2" t="s" s="9">
+        <v>68</v>
+      </c>
+      <c r="AL2" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="AM2" t="s" s="8">
+        <v>70</v>
+      </c>
+      <c r="AN2" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="AO2" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="AP2" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="AQ2" t="s" s="9">
+        <v>74</v>
+      </c>
+      <c r="AR2" t="s" s="6">
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="22.55" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>59</v>
+      <c r="A3" t="s" s="3">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>45</v>
       </c>
       <c r="C3" t="s" s="10">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D3" s="11">
         <v>12345678</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="G3" t="b" s="13">
         <v>0</v>
@@ -1767,90 +1902,252 @@
         <v>0</v>
       </c>
       <c r="I3" t="s" s="12">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s" s="12">
+        <v>50</v>
+      </c>
+      <c r="K3" t="s" s="12">
+        <v>50</v>
+      </c>
+      <c r="L3" t="s" s="12">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s" s="12">
+        <v>52</v>
+      </c>
+      <c r="N3" t="s" s="12">
+        <v>53</v>
+      </c>
+      <c r="O3" t="s" s="12">
+        <v>54</v>
+      </c>
+      <c r="P3" t="s" s="12">
+        <v>55</v>
+      </c>
+      <c r="Q3" t="s" s="12">
+        <v>56</v>
+      </c>
+      <c r="R3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="S3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="T3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="U3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="V3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="W3" t="s" s="12">
+        <v>58</v>
+      </c>
+      <c r="X3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="Y3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="Z3" t="s" s="12">
+        <v>59</v>
+      </c>
+      <c r="AA3" t="s" s="12">
+        <v>60</v>
+      </c>
+      <c r="AB3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="AC3" t="s" s="12">
+        <v>61</v>
+      </c>
+      <c r="AD3" t="s" s="12">
+        <v>62</v>
+      </c>
+      <c r="AE3" t="s" s="12">
+        <v>57</v>
+      </c>
+      <c r="AF3" t="s" s="12">
         <v>63</v>
       </c>
-      <c r="J3" t="s" s="12">
-        <v>41</v>
-      </c>
-      <c r="K3" t="s" s="12">
-        <v>41</v>
-      </c>
-      <c r="L3" t="s" s="12">
-        <v>42</v>
-      </c>
-      <c r="M3" t="s" s="12">
-        <v>43</v>
-      </c>
-      <c r="N3" t="s" s="12">
-        <v>44</v>
-      </c>
-      <c r="O3" t="s" s="12">
+      <c r="AG3" t="s" s="12">
         <v>64</v>
       </c>
-      <c r="P3" t="s" s="12">
-        <v>65</v>
-      </c>
-      <c r="Q3" t="s" s="12">
+      <c r="AH3" t="s" s="8">
+        <v>77</v>
+      </c>
+      <c r="AI3" t="s" s="8">
         <v>66</v>
       </c>
-      <c r="R3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="S3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="T3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="U3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="V3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="W3" t="s" s="12">
+      <c r="AJ3" t="s" s="8">
         <v>67</v>
       </c>
-      <c r="X3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="Y3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="Z3" t="s" s="12">
+      <c r="AK3" t="s" s="14">
         <v>68</v>
       </c>
-      <c r="AA3" t="s" s="12">
+      <c r="AL3" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="AM3" t="s" s="8">
+        <v>70</v>
+      </c>
+      <c r="AN3" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="AO3" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="AP3" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="AQ3" t="s" s="14">
+        <v>74</v>
+      </c>
+      <c r="AR3" t="s" s="12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" ht="22.55" customHeight="1">
+      <c r="A4" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s" s="16">
+        <v>80</v>
+      </c>
+      <c r="D4" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E4" t="s" s="6">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s" s="6">
+        <v>82</v>
+      </c>
+      <c r="G4" t="b" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s" s="6">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s" s="6">
+        <v>50</v>
+      </c>
+      <c r="K4" t="s" s="6">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s" s="6">
         <v>51</v>
       </c>
-      <c r="AB3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="AC3" t="s" s="12">
+      <c r="M4" t="s" s="6">
         <v>52</v>
       </c>
-      <c r="AD3" t="s" s="12">
+      <c r="N4" t="s" s="6">
+        <v>53</v>
+      </c>
+      <c r="O4" t="s" s="6">
+        <v>84</v>
+      </c>
+      <c r="P4" t="s" s="6">
+        <v>85</v>
+      </c>
+      <c r="Q4" t="s" s="6">
+        <v>86</v>
+      </c>
+      <c r="R4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="S4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="T4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="U4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="V4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="W4" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="X4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="Z4" t="s" s="6">
+        <v>88</v>
+      </c>
+      <c r="AA4" t="s" s="6">
+        <v>60</v>
+      </c>
+      <c r="AB4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="AC4" t="s" s="6">
+        <v>61</v>
+      </c>
+      <c r="AD4" t="s" s="6">
+        <v>89</v>
+      </c>
+      <c r="AE4" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="AF4" t="s" s="6">
+        <v>63</v>
+      </c>
+      <c r="AG4" t="s" s="6">
+        <v>64</v>
+      </c>
+      <c r="AH4" t="s" s="9">
+        <v>77</v>
+      </c>
+      <c r="AI4" t="s" s="9">
+        <v>66</v>
+      </c>
+      <c r="AJ4" t="s" s="9">
+        <v>67</v>
+      </c>
+      <c r="AK4" t="s" s="9">
+        <v>68</v>
+      </c>
+      <c r="AL4" t="s" s="9">
         <v>69</v>
       </c>
-      <c r="AE3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="AF3" t="s" s="12">
-        <v>54</v>
-      </c>
-      <c r="AG3" t="s" s="12">
-        <v>55</v>
-      </c>
-      <c r="AH3" t="s" s="14">
-        <v>56</v>
-      </c>
-      <c r="AI3" t="s" s="12">
-        <v>57</v>
+      <c r="AM4" t="s" s="9">
+        <v>70</v>
+      </c>
+      <c r="AN4" t="s" s="9">
+        <v>71</v>
+      </c>
+      <c r="AO4" t="s" s="9">
+        <v>72</v>
+      </c>
+      <c r="AP4" t="s" s="9">
+        <v>73</v>
+      </c>
+      <c r="AQ4" t="s" s="9">
+        <v>74</v>
+      </c>
+      <c r="AR4" t="s" s="6">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="qa1@gogotech.hk "/>
+    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="qa1@gogotech.hk "/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
update delivery page automation
added the packageInfo page automation
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -137,6 +137,30 @@
   </si>
   <si>
     <t>RECIPIENT_PHONE_NUMBER</t>
+  </si>
+  <si>
+    <t>DROP_OFF_TIME</t>
+  </si>
+  <si>
+    <t>CONTENT_TYPE</t>
+  </si>
+  <si>
+    <t>SIZE</t>
+  </si>
+  <si>
+    <t>WEIGHT</t>
+  </si>
+  <si>
+    <t>BUY_FLAG</t>
+  </si>
+  <si>
+    <t>BUY_OPTION</t>
+  </si>
+  <si>
+    <t>REMARKS_FLAG</t>
+  </si>
+  <si>
+    <t>DELIVERY_REMARKS</t>
   </si>
   <si>
     <t>DRIVER_PHONE_NUMBER</t>
@@ -251,6 +275,24 @@
     <t>53326890</t>
   </si>
   <si>
+    <t>Instant</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Testing delivery notes</t>
+  </si>
+  <si>
     <t>66778899</t>
   </si>
   <si>
@@ -260,6 +302,17 @@
     <t>TC002_Complete a transport order with testing personal account</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>qa1@gogotech.hk</t>
+    </r>
+  </si>
+  <si>
     <t>T</t>
   </si>
   <si>
@@ -269,7 +322,15 @@
     <t>Business</t>
   </si>
   <si>
-    <t>qadmaster1@gogotech.hk</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>qadmaster1@gogotech.hk</t>
+    </r>
   </si>
   <si>
     <t>Ma On Shan</t>
@@ -282,12 +343,6 @@
   </si>
   <si>
     <t>Standard</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>Lion Rock Tunnel</t>
@@ -306,7 +361,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -339,6 +394,23 @@
       <color indexed="8"/>
       <name val="Times Roman"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="14"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="15"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -360,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -394,28 +466,13 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -439,52 +496,69 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,7 +568,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -519,32 +593,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,6 +656,9 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ee"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1598,14 +1690,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AZ4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="44" width="16.3516" style="1" customWidth="1"/>
-    <col min="45" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="52" width="16.3516" style="1" customWidth="1"/>
+    <col min="53" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
@@ -1741,25 +1833,49 @@
       <c r="AR1" t="s" s="2">
         <v>43</v>
       </c>
+      <c r="AS1" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s" s="2">
+        <v>51</v>
+      </c>
     </row>
     <row r="2" ht="22.55" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D2" s="5">
         <v>12345678</v>
       </c>
       <c r="E2" t="s" s="6">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s" s="6">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G2" t="b" s="7">
         <v>0</v>
@@ -1768,386 +1884,459 @@
         <v>0</v>
       </c>
       <c r="I2" t="s" s="6">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s" s="6">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s" s="6">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s" s="6">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s" s="6">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="N2" t="s" s="6">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="O2" t="s" s="6">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="P2" t="s" s="6">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="Q2" t="s" s="6">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="R2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="S2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="T2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="U2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="V2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="W2" t="s" s="6">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="X2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="Y2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="Z2" t="s" s="6">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="AA2" t="s" s="6">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="AB2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="AC2" t="s" s="6">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="AD2" t="s" s="6">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="AE2" t="s" s="6">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="AF2" t="s" s="6">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="AG2" t="s" s="6">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="AH2" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="AI2" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="AJ2" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="AK2" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="AL2" t="s" s="8">
+        <v>77</v>
+      </c>
+      <c r="AM2" t="s" s="8">
+        <v>78</v>
+      </c>
+      <c r="AN2" t="s" s="8">
+        <v>79</v>
+      </c>
+      <c r="AO2" t="s" s="8">
+        <v>80</v>
+      </c>
+      <c r="AP2" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="AQ2" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="AR2" t="s" s="8">
+        <v>83</v>
+      </c>
+      <c r="AS2" t="s" s="8">
+        <v>84</v>
+      </c>
+      <c r="AT2" t="s" s="8">
+        <v>85</v>
+      </c>
+      <c r="AU2" t="s" s="8">
         <v>65</v>
       </c>
-      <c r="AI2" t="s" s="8">
-        <v>66</v>
-      </c>
-      <c r="AJ2" t="s" s="8">
-        <v>67</v>
-      </c>
-      <c r="AK2" t="s" s="9">
-        <v>68</v>
-      </c>
-      <c r="AL2" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="AM2" t="s" s="8">
-        <v>70</v>
-      </c>
-      <c r="AN2" t="s" s="8">
-        <v>71</v>
-      </c>
-      <c r="AO2" t="s" s="8">
-        <v>72</v>
-      </c>
-      <c r="AP2" t="s" s="8">
-        <v>73</v>
-      </c>
-      <c r="AQ2" t="s" s="9">
-        <v>74</v>
-      </c>
-      <c r="AR2" t="s" s="6">
-        <v>75</v>
+      <c r="AV2" t="s" s="8">
+        <v>86</v>
+      </c>
+      <c r="AW2" t="s" s="8">
+        <v>65</v>
+      </c>
+      <c r="AX2" t="s" s="8">
+        <v>87</v>
+      </c>
+      <c r="AY2" t="s" s="8">
+        <v>88</v>
+      </c>
+      <c r="AZ2" t="s" s="6">
+        <v>89</v>
       </c>
     </row>
     <row r="3" ht="22.55" customHeight="1">
-      <c r="A3" t="s" s="3">
+      <c r="A3" t="s" s="9">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s" s="11">
+        <v>91</v>
+      </c>
+      <c r="D3" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="E3" t="s" s="10">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="G3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s" s="10">
+        <v>57</v>
+      </c>
+      <c r="J3" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="L3" t="s" s="10">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s" s="10">
+        <v>60</v>
+      </c>
+      <c r="N3" t="s" s="10">
+        <v>61</v>
+      </c>
+      <c r="O3" t="s" s="10">
+        <v>62</v>
+      </c>
+      <c r="P3" s="13">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="13">
+        <v>2</v>
+      </c>
+      <c r="R3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="V3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s" s="10">
+        <v>66</v>
+      </c>
+      <c r="X3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s" s="10">
+        <v>67</v>
+      </c>
+      <c r="AA3" s="13">
+        <v>51112222</v>
+      </c>
+      <c r="AB3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="13">
+        <v>852</v>
+      </c>
+      <c r="AD3" s="13">
+        <v>20</v>
+      </c>
+      <c r="AE3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="AG3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="s" s="14">
+        <v>92</v>
+      </c>
+      <c r="AI3" t="s" s="14">
+        <v>74</v>
+      </c>
+      <c r="AJ3" t="s" s="14">
+        <v>75</v>
+      </c>
+      <c r="AK3" t="s" s="14">
         <v>76</v>
       </c>
-      <c r="B3" t="s" s="3">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>46</v>
-      </c>
-      <c r="D3" s="11">
-        <v>12345678</v>
-      </c>
-      <c r="E3" t="s" s="12">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s" s="12">
-        <v>48</v>
-      </c>
-      <c r="G3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s" s="12">
-        <v>49</v>
-      </c>
-      <c r="J3" t="s" s="12">
-        <v>50</v>
-      </c>
-      <c r="K3" t="s" s="12">
-        <v>50</v>
-      </c>
-      <c r="L3" t="s" s="12">
-        <v>51</v>
-      </c>
-      <c r="M3" t="s" s="12">
-        <v>52</v>
-      </c>
-      <c r="N3" t="s" s="12">
-        <v>53</v>
-      </c>
-      <c r="O3" t="s" s="12">
-        <v>54</v>
-      </c>
-      <c r="P3" t="s" s="12">
-        <v>55</v>
-      </c>
-      <c r="Q3" t="s" s="12">
-        <v>56</v>
-      </c>
-      <c r="R3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="S3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="T3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="U3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="V3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="W3" t="s" s="12">
-        <v>58</v>
-      </c>
-      <c r="X3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="Y3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="Z3" t="s" s="12">
-        <v>59</v>
-      </c>
-      <c r="AA3" t="s" s="12">
-        <v>60</v>
-      </c>
-      <c r="AB3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="AC3" t="s" s="12">
-        <v>61</v>
-      </c>
-      <c r="AD3" t="s" s="12">
-        <v>62</v>
-      </c>
-      <c r="AE3" t="s" s="12">
-        <v>57</v>
-      </c>
-      <c r="AF3" t="s" s="12">
-        <v>63</v>
-      </c>
-      <c r="AG3" t="s" s="12">
-        <v>64</v>
-      </c>
-      <c r="AH3" t="s" s="8">
-        <v>77</v>
-      </c>
-      <c r="AI3" t="s" s="8">
-        <v>66</v>
-      </c>
-      <c r="AJ3" t="s" s="8">
-        <v>67</v>
-      </c>
-      <c r="AK3" t="s" s="14">
-        <v>68</v>
-      </c>
-      <c r="AL3" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="AM3" t="s" s="8">
-        <v>70</v>
-      </c>
-      <c r="AN3" t="s" s="8">
-        <v>71</v>
-      </c>
-      <c r="AO3" t="s" s="8">
-        <v>72</v>
-      </c>
-      <c r="AP3" t="s" s="8">
-        <v>73</v>
+      <c r="AL3" s="12">
+        <v>92516783</v>
+      </c>
+      <c r="AM3" t="s" s="14">
+        <v>78</v>
+      </c>
+      <c r="AN3" t="s" s="14">
+        <v>79</v>
+      </c>
+      <c r="AO3" t="s" s="14">
+        <v>80</v>
+      </c>
+      <c r="AP3" s="12">
+        <v>53326890</v>
       </c>
       <c r="AQ3" t="s" s="14">
-        <v>74</v>
-      </c>
-      <c r="AR3" t="s" s="12">
-        <v>75</v>
+        <v>82</v>
+      </c>
+      <c r="AR3" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="AS3" s="12">
+        <v>30</v>
+      </c>
+      <c r="AT3" s="12">
+        <v>15</v>
+      </c>
+      <c r="AU3" t="b" s="12">
+        <v>1</v>
+      </c>
+      <c r="AV3" s="12">
+        <v>1000</v>
+      </c>
+      <c r="AW3" t="b" s="12">
+        <v>1</v>
+      </c>
+      <c r="AX3" t="s" s="14">
+        <v>87</v>
+      </c>
+      <c r="AY3" s="12">
+        <v>66778899</v>
+      </c>
+      <c r="AZ3" t="s" s="15">
+        <v>89</v>
       </c>
     </row>
     <row r="4" ht="22.55" customHeight="1">
-      <c r="A4" t="s" s="15">
+      <c r="A4" t="s" s="16">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s" s="17">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s" s="17">
+        <v>95</v>
+      </c>
+      <c r="D4" s="18">
+        <v>12345678</v>
+      </c>
+      <c r="E4" t="s" s="17">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s" s="17">
+        <v>97</v>
+      </c>
+      <c r="G4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s" s="17">
+        <v>98</v>
+      </c>
+      <c r="J4" t="s" s="17">
+        <v>58</v>
+      </c>
+      <c r="K4" t="s" s="17">
+        <v>58</v>
+      </c>
+      <c r="L4" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="M4" t="s" s="17">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s" s="17">
+        <v>61</v>
+      </c>
+      <c r="O4" t="s" s="17">
+        <v>99</v>
+      </c>
+      <c r="P4" s="19">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>1</v>
+      </c>
+      <c r="R4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="S4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="T4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="U4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="V4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s" s="17">
+        <v>100</v>
+      </c>
+      <c r="X4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s" s="17">
+        <v>101</v>
+      </c>
+      <c r="AA4" s="19">
+        <v>51112222</v>
+      </c>
+      <c r="AB4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="19">
+        <v>852</v>
+      </c>
+      <c r="AD4" t="s" s="17">
+        <v>102</v>
+      </c>
+      <c r="AE4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="s" s="17">
+        <v>71</v>
+      </c>
+      <c r="AG4" t="b" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="s" s="20">
+        <v>92</v>
+      </c>
+      <c r="AI4" t="s" s="20">
+        <v>74</v>
+      </c>
+      <c r="AJ4" t="s" s="20">
+        <v>75</v>
+      </c>
+      <c r="AK4" t="s" s="20">
+        <v>76</v>
+      </c>
+      <c r="AL4" s="18">
+        <v>92516783</v>
+      </c>
+      <c r="AM4" t="s" s="20">
         <v>78</v>
       </c>
-      <c r="B4" t="s" s="15">
+      <c r="AN4" t="s" s="20">
         <v>79</v>
       </c>
-      <c r="C4" t="s" s="16">
+      <c r="AO4" t="s" s="20">
         <v>80</v>
       </c>
-      <c r="D4" s="5">
-        <v>12345678</v>
-      </c>
-      <c r="E4" t="s" s="6">
-        <v>81</v>
-      </c>
-      <c r="F4" t="s" s="6">
+      <c r="AP4" s="18">
+        <v>53326890</v>
+      </c>
+      <c r="AQ4" t="s" s="20">
         <v>82</v>
       </c>
-      <c r="G4" t="b" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s" s="6">
+      <c r="AR4" t="s" s="20">
         <v>83</v>
       </c>
-      <c r="J4" t="s" s="6">
-        <v>50</v>
-      </c>
-      <c r="K4" t="s" s="6">
-        <v>50</v>
-      </c>
-      <c r="L4" t="s" s="6">
-        <v>51</v>
-      </c>
-      <c r="M4" t="s" s="6">
-        <v>52</v>
-      </c>
-      <c r="N4" t="s" s="6">
-        <v>53</v>
-      </c>
-      <c r="O4" t="s" s="6">
-        <v>84</v>
-      </c>
-      <c r="P4" t="s" s="6">
-        <v>85</v>
-      </c>
-      <c r="Q4" t="s" s="6">
-        <v>86</v>
-      </c>
-      <c r="R4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="S4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="T4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="U4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="V4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="W4" t="s" s="6">
+      <c r="AS4" s="18">
+        <v>30</v>
+      </c>
+      <c r="AT4" s="18">
+        <v>15</v>
+      </c>
+      <c r="AU4" t="b" s="18">
+        <v>1</v>
+      </c>
+      <c r="AV4" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AW4" t="b" s="18">
+        <v>1</v>
+      </c>
+      <c r="AX4" t="s" s="20">
         <v>87</v>
       </c>
-      <c r="X4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="Y4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="Z4" t="s" s="6">
-        <v>88</v>
-      </c>
-      <c r="AA4" t="s" s="6">
-        <v>60</v>
-      </c>
-      <c r="AB4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="AC4" t="s" s="6">
-        <v>61</v>
-      </c>
-      <c r="AD4" t="s" s="6">
+      <c r="AY4" s="18">
+        <v>66778899</v>
+      </c>
+      <c r="AZ4" t="s" s="21">
         <v>89</v>
-      </c>
-      <c r="AE4" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="AF4" t="s" s="6">
-        <v>63</v>
-      </c>
-      <c r="AG4" t="s" s="6">
-        <v>64</v>
-      </c>
-      <c r="AH4" t="s" s="9">
-        <v>77</v>
-      </c>
-      <c r="AI4" t="s" s="9">
-        <v>66</v>
-      </c>
-      <c r="AJ4" t="s" s="9">
-        <v>67</v>
-      </c>
-      <c r="AK4" t="s" s="9">
-        <v>68</v>
-      </c>
-      <c r="AL4" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="AM4" t="s" s="9">
-        <v>70</v>
-      </c>
-      <c r="AN4" t="s" s="9">
-        <v>71</v>
-      </c>
-      <c r="AO4" t="s" s="9">
-        <v>72</v>
-      </c>
-      <c r="AP4" t="s" s="9">
-        <v>73</v>
-      </c>
-      <c r="AQ4" t="s" s="9">
-        <v>74</v>
-      </c>
-      <c r="AR4" t="s" s="6">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="qa1@gogotech.hk "/>
-    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="qa1@gogotech.hk "/>
+    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="qa1@gogotech.hk"/>
+    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display="qadmaster1@gogotech.hk"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
update the delivery order process
finish the delivery order process and requires further modify it
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -224,6 +224,9 @@
     <t>2</t>
   </si>
   <si>
+    <t>TRUE</t>
+  </si>
+  <si>
     <t>FALSE</t>
   </si>
   <si>
@@ -245,13 +248,10 @@
     <t>CASH</t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
-    <t>North Point</t>
+    <t>Sai Wan Ho</t>
   </si>
   <si>
     <t>3026A</t>
@@ -263,7 +263,7 @@
     <t>92516783</t>
   </si>
   <si>
-    <t>Siu Sai Wan</t>
+    <t>Wan Chai</t>
   </si>
   <si>
     <t>4218B</t>
@@ -297,61 +297,6 @@
   </si>
   <si>
     <t>Aa123456</t>
-  </si>
-  <si>
-    <t>TC002_Complete a transport order with testing personal account</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="15"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>qa1@gogotech.hk</t>
-    </r>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>TC003_Complete a transport order with testing business account</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="15"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>qadmaster1@gogotech.hk</t>
-    </r>
-  </si>
-  <si>
-    <t>Ma On Shan</t>
-  </si>
-  <si>
-    <t>Festival walk</t>
-  </si>
-  <si>
-    <t>Cityu</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>Lion Rock Tunnel</t>
-  </si>
-  <si>
-    <t>QA Tester</t>
-  </si>
-  <si>
-    <t>No tip</t>
   </si>
 </sst>
 </file>
@@ -361,7 +306,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -394,23 +339,6 @@
       <color indexed="8"/>
       <name val="Times Roman"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color indexed="14"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color indexed="15"/>
-      <name val="Helvetica Neue"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -432,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -500,75 +428,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -596,45 +462,6 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,9 +483,6 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ee"/>
-      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1690,7 +1514,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AZ4"/>
+  <dimension ref="A1:AZ2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1917,46 +1741,46 @@
         <v>65</v>
       </c>
       <c r="T2" t="s" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U2" t="s" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V2" t="s" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W2" t="s" s="6">
+        <v>67</v>
+      </c>
+      <c r="X2" t="s" s="6">
         <v>66</v>
       </c>
-      <c r="X2" t="s" s="6">
-        <v>65</v>
-      </c>
       <c r="Y2" t="s" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Z2" t="s" s="6">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA2" t="s" s="6">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AB2" t="s" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AC2" t="s" s="6">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD2" t="s" s="6">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AE2" t="s" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AF2" t="s" s="6">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AG2" t="s" s="6">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="AH2" t="s" s="8">
         <v>73</v>
@@ -1998,13 +1822,13 @@
         <v>85</v>
       </c>
       <c r="AU2" t="s" s="8">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AV2" t="s" s="8">
         <v>86</v>
       </c>
       <c r="AW2" t="s" s="8">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AX2" t="s" s="8">
         <v>87</v>
@@ -2013,330 +1837,12 @@
         <v>88</v>
       </c>
       <c r="AZ2" t="s" s="6">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" ht="22.55" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s" s="11">
-        <v>91</v>
-      </c>
-      <c r="D3" s="12">
-        <v>12345678</v>
-      </c>
-      <c r="E3" t="s" s="10">
-        <v>55</v>
-      </c>
-      <c r="F3" t="s" s="10">
-        <v>56</v>
-      </c>
-      <c r="G3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s" s="10">
-        <v>57</v>
-      </c>
-      <c r="J3" t="s" s="10">
-        <v>58</v>
-      </c>
-      <c r="K3" t="s" s="10">
-        <v>58</v>
-      </c>
-      <c r="L3" t="s" s="10">
-        <v>59</v>
-      </c>
-      <c r="M3" t="s" s="10">
-        <v>60</v>
-      </c>
-      <c r="N3" t="s" s="10">
-        <v>61</v>
-      </c>
-      <c r="O3" t="s" s="10">
-        <v>62</v>
-      </c>
-      <c r="P3" s="13">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="13">
-        <v>2</v>
-      </c>
-      <c r="R3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="S3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="T3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="U3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="V3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="W3" t="s" s="10">
-        <v>66</v>
-      </c>
-      <c r="X3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="s" s="10">
-        <v>67</v>
-      </c>
-      <c r="AA3" s="13">
-        <v>51112222</v>
-      </c>
-      <c r="AB3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="13">
-        <v>852</v>
-      </c>
-      <c r="AD3" s="13">
-        <v>20</v>
-      </c>
-      <c r="AE3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="AF3" t="s" s="10">
-        <v>71</v>
-      </c>
-      <c r="AG3" t="b" s="13">
-        <v>0</v>
-      </c>
-      <c r="AH3" t="s" s="14">
-        <v>92</v>
-      </c>
-      <c r="AI3" t="s" s="14">
-        <v>74</v>
-      </c>
-      <c r="AJ3" t="s" s="14">
-        <v>75</v>
-      </c>
-      <c r="AK3" t="s" s="14">
-        <v>76</v>
-      </c>
-      <c r="AL3" s="12">
-        <v>92516783</v>
-      </c>
-      <c r="AM3" t="s" s="14">
-        <v>78</v>
-      </c>
-      <c r="AN3" t="s" s="14">
-        <v>79</v>
-      </c>
-      <c r="AO3" t="s" s="14">
-        <v>80</v>
-      </c>
-      <c r="AP3" s="12">
-        <v>53326890</v>
-      </c>
-      <c r="AQ3" t="s" s="14">
-        <v>82</v>
-      </c>
-      <c r="AR3" t="s" s="14">
-        <v>83</v>
-      </c>
-      <c r="AS3" s="12">
-        <v>30</v>
-      </c>
-      <c r="AT3" s="12">
-        <v>15</v>
-      </c>
-      <c r="AU3" t="b" s="12">
-        <v>1</v>
-      </c>
-      <c r="AV3" s="12">
-        <v>1000</v>
-      </c>
-      <c r="AW3" t="b" s="12">
-        <v>1</v>
-      </c>
-      <c r="AX3" t="s" s="14">
-        <v>87</v>
-      </c>
-      <c r="AY3" s="12">
-        <v>66778899</v>
-      </c>
-      <c r="AZ3" t="s" s="15">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" ht="22.55" customHeight="1">
-      <c r="A4" t="s" s="16">
-        <v>93</v>
-      </c>
-      <c r="B4" t="s" s="17">
-        <v>94</v>
-      </c>
-      <c r="C4" t="s" s="17">
-        <v>95</v>
-      </c>
-      <c r="D4" s="18">
-        <v>12345678</v>
-      </c>
-      <c r="E4" t="s" s="17">
-        <v>96</v>
-      </c>
-      <c r="F4" t="s" s="17">
-        <v>97</v>
-      </c>
-      <c r="G4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s" s="17">
-        <v>98</v>
-      </c>
-      <c r="J4" t="s" s="17">
-        <v>58</v>
-      </c>
-      <c r="K4" t="s" s="17">
-        <v>58</v>
-      </c>
-      <c r="L4" t="s" s="17">
-        <v>59</v>
-      </c>
-      <c r="M4" t="s" s="17">
-        <v>60</v>
-      </c>
-      <c r="N4" t="s" s="17">
-        <v>61</v>
-      </c>
-      <c r="O4" t="s" s="17">
-        <v>99</v>
-      </c>
-      <c r="P4" s="19">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="19">
-        <v>1</v>
-      </c>
-      <c r="R4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="S4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="T4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="U4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="V4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="W4" t="s" s="17">
-        <v>100</v>
-      </c>
-      <c r="X4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="s" s="17">
-        <v>101</v>
-      </c>
-      <c r="AA4" s="19">
-        <v>51112222</v>
-      </c>
-      <c r="AB4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="19">
-        <v>852</v>
-      </c>
-      <c r="AD4" t="s" s="17">
-        <v>102</v>
-      </c>
-      <c r="AE4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="s" s="17">
-        <v>71</v>
-      </c>
-      <c r="AG4" t="b" s="19">
-        <v>0</v>
-      </c>
-      <c r="AH4" t="s" s="20">
-        <v>92</v>
-      </c>
-      <c r="AI4" t="s" s="20">
-        <v>74</v>
-      </c>
-      <c r="AJ4" t="s" s="20">
-        <v>75</v>
-      </c>
-      <c r="AK4" t="s" s="20">
-        <v>76</v>
-      </c>
-      <c r="AL4" s="18">
-        <v>92516783</v>
-      </c>
-      <c r="AM4" t="s" s="20">
-        <v>78</v>
-      </c>
-      <c r="AN4" t="s" s="20">
-        <v>79</v>
-      </c>
-      <c r="AO4" t="s" s="20">
-        <v>80</v>
-      </c>
-      <c r="AP4" s="18">
-        <v>53326890</v>
-      </c>
-      <c r="AQ4" t="s" s="20">
-        <v>82</v>
-      </c>
-      <c r="AR4" t="s" s="20">
-        <v>83</v>
-      </c>
-      <c r="AS4" s="18">
-        <v>30</v>
-      </c>
-      <c r="AT4" s="18">
-        <v>15</v>
-      </c>
-      <c r="AU4" t="b" s="18">
-        <v>1</v>
-      </c>
-      <c r="AV4" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AW4" t="b" s="18">
-        <v>1</v>
-      </c>
-      <c r="AX4" t="s" s="20">
-        <v>87</v>
-      </c>
-      <c r="AY4" s="18">
-        <v>66778899</v>
-      </c>
-      <c r="AZ4" t="s" s="21">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="qa1@gogotech.hk "/>
-    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="qa1@gogotech.hk"/>
-    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display="qadmaster1@gogotech.hk"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
update delivery order in business account
adding until the merchant details
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -5,13 +5,13 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -163,35 +163,25 @@
     <t>DELIVERY_REMARKS</t>
   </si>
   <si>
+    <t>MERCHANT_ORDER_FLAG</t>
+  </si>
+  <si>
+    <t>MERCHANT_REMARKS</t>
+  </si>
+  <si>
     <t>DRIVER_PHONE_NUMBER</t>
   </si>
   <si>
     <t>DRIVER_PASSWORD</t>
   </si>
   <si>
-    <t>TC001_Complete a delivery order with testing personal account</t>
-  </si>
-  <si>
-    <t>Personal</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>qa1@gogotech.hk</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t>TC001_Complete a delivery order with testing business account</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>qadmaster1@gogotech.hk</t>
   </si>
   <si>
     <t>Tin Hau</t>
@@ -218,40 +208,19 @@
     <t>Basic</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
     <t>Tai Lam Tunnel</t>
   </si>
   <si>
     <t>William Koh</t>
   </si>
   <si>
-    <t>51112222</t>
-  </si>
-  <si>
-    <t>852</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>CASH</t>
   </si>
   <si>
     <t>D</t>
   </si>
   <si>
-    <t>Sai Wan Ho</t>
+    <t>North Point</t>
   </si>
   <si>
     <t>3026A</t>
@@ -260,10 +229,7 @@
     <t>William</t>
   </si>
   <si>
-    <t>92516783</t>
-  </si>
-  <si>
-    <t>Wan Chai</t>
+    <t>Chai Wan</t>
   </si>
   <si>
     <t>4218B</t>
@@ -272,28 +238,16 @@
     <t>William2</t>
   </si>
   <si>
-    <t>53326890</t>
-  </si>
-  <si>
     <t>Instant</t>
   </si>
   <si>
     <t>Electronics</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>Testing delivery notes</t>
   </si>
   <si>
-    <t>66778899</t>
+    <t>Testing merchant order remarks</t>
   </si>
   <si>
     <t>Aa123456</t>
@@ -310,7 +264,7 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
@@ -324,23 +278,22 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="10"/>
+      <sz val="8"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="10"/>
+      <sz val="8"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <color indexed="8"/>
       <name val="Times Roman"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,14 +306,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -379,51 +326,6 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
@@ -431,36 +333,30 @@
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,19 +375,17 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Blank">
+    <a:clrScheme name="Sheets">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -505,22 +399,22 @@
         <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="00A2FF"/>
+        <a:srgbClr val="4285F4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="16E7CF"/>
+        <a:srgbClr val="EA4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="61D836"/>
+        <a:srgbClr val="FBBC04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFD932"/>
+        <a:srgbClr val="34A853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF644E"/>
+        <a:srgbClr val="FF6D01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="FF42A1"/>
+        <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -529,7 +423,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Blank">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
         <a:latin typeface="Helvetica Neue"/>
         <a:ea typeface="Helvetica Neue"/>
@@ -541,7 +435,7 @@
         <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Blank">
+    <a:fmtScheme name="Sheets">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -681,17 +575,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -718,10 +612,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Arial"/>
+            <a:ea typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+            <a:sym typeface="Arial"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -960,12 +854,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1242,7 +1136,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1269,10 +1163,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Arial"/>
+            <a:ea typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+            <a:sym typeface="Arial"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1514,17 +1408,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AZ2"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:BB2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="52" width="16.3516" style="1" customWidth="1"/>
-    <col min="53" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="54" width="12.6719" style="1" customWidth="1"/>
+    <col min="55" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32.25" customHeight="1">
+    <row r="1" ht="13" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1681,171 +1578,180 @@
       <c r="AZ1" t="s" s="2">
         <v>51</v>
       </c>
+      <c r="BA1" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s" s="2">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" ht="22.55" customHeight="1">
+    <row r="2" ht="14" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>54</v>
-      </c>
-      <c r="D2" s="5">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="D2" s="4">
         <v>12345678</v>
       </c>
-      <c r="E2" t="s" s="6">
-        <v>55</v>
-      </c>
-      <c r="F2" t="s" s="6">
-        <v>56</v>
-      </c>
-      <c r="G2" t="b" s="7">
+      <c r="E2" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="G2" t="b" s="5">
         <v>0</v>
       </c>
-      <c r="H2" t="b" s="7">
+      <c r="H2" t="b" s="5">
         <v>0</v>
       </c>
-      <c r="I2" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="J2" t="s" s="6">
-        <v>58</v>
-      </c>
-      <c r="K2" t="s" s="6">
-        <v>58</v>
-      </c>
-      <c r="L2" t="s" s="6">
+      <c r="I2" t="s" s="3">
         <v>59</v>
       </c>
-      <c r="M2" t="s" s="6">
+      <c r="J2" t="s" s="3">
         <v>60</v>
       </c>
-      <c r="N2" t="s" s="6">
+      <c r="K2" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="L2" t="s" s="3">
         <v>61</v>
       </c>
-      <c r="O2" t="s" s="6">
+      <c r="M2" t="s" s="3">
         <v>62</v>
       </c>
-      <c r="P2" t="s" s="6">
+      <c r="N2" t="s" s="3">
         <v>63</v>
       </c>
-      <c r="Q2" t="s" s="6">
+      <c r="O2" t="s" s="3">
         <v>64</v>
       </c>
-      <c r="R2" t="s" s="6">
+      <c r="P2" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>2</v>
+      </c>
+      <c r="R2" t="b" s="5">
+        <v>1</v>
+      </c>
+      <c r="S2" t="b" s="5">
+        <v>1</v>
+      </c>
+      <c r="T2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="V2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s" s="3">
         <v>65</v>
       </c>
-      <c r="S2" t="s" s="6">
-        <v>65</v>
-      </c>
-      <c r="T2" t="s" s="6">
+      <c r="X2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s" s="3">
         <v>66</v>
       </c>
-      <c r="U2" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="V2" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="W2" t="s" s="6">
+      <c r="AA2" s="5">
+        <v>51112222</v>
+      </c>
+      <c r="AB2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>852</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>20</v>
+      </c>
+      <c r="AE2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="s" s="3">
         <v>67</v>
       </c>
-      <c r="X2" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="Y2" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="Z2" t="s" s="6">
+      <c r="AG2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="s" s="6">
         <v>68</v>
       </c>
-      <c r="AA2" t="s" s="6">
+      <c r="AI2" t="s" s="6">
         <v>69</v>
       </c>
-      <c r="AB2" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="AC2" t="s" s="6">
+      <c r="AJ2" t="s" s="6">
         <v>70</v>
       </c>
-      <c r="AD2" t="s" s="6">
+      <c r="AK2" t="s" s="6">
         <v>71</v>
       </c>
-      <c r="AE2" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="AF2" t="s" s="6">
+      <c r="AL2" s="4">
+        <v>92516783</v>
+      </c>
+      <c r="AM2" t="s" s="6">
         <v>72</v>
       </c>
-      <c r="AG2" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="AH2" t="s" s="8">
+      <c r="AN2" t="s" s="6">
         <v>73</v>
       </c>
-      <c r="AI2" t="s" s="8">
+      <c r="AO2" t="s" s="6">
         <v>74</v>
       </c>
-      <c r="AJ2" t="s" s="8">
+      <c r="AP2" s="4">
+        <v>53326890</v>
+      </c>
+      <c r="AQ2" t="s" s="6">
         <v>75</v>
       </c>
-      <c r="AK2" t="s" s="8">
+      <c r="AR2" t="s" s="6">
         <v>76</v>
       </c>
-      <c r="AL2" t="s" s="8">
+      <c r="AS2" s="4">
+        <v>30</v>
+      </c>
+      <c r="AT2" s="4">
+        <v>15</v>
+      </c>
+      <c r="AU2" t="b" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AW2" t="b" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="s" s="6">
         <v>77</v>
       </c>
-      <c r="AM2" t="s" s="8">
+      <c r="AY2" t="b" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ2" t="s" s="6">
         <v>78</v>
       </c>
-      <c r="AN2" t="s" s="8">
+      <c r="BA2" s="4">
+        <v>66778899</v>
+      </c>
+      <c r="BB2" t="s" s="3">
         <v>79</v>
-      </c>
-      <c r="AO2" t="s" s="8">
-        <v>80</v>
-      </c>
-      <c r="AP2" t="s" s="8">
-        <v>81</v>
-      </c>
-      <c r="AQ2" t="s" s="8">
-        <v>82</v>
-      </c>
-      <c r="AR2" t="s" s="8">
-        <v>83</v>
-      </c>
-      <c r="AS2" t="s" s="8">
-        <v>84</v>
-      </c>
-      <c r="AT2" t="s" s="8">
-        <v>85</v>
-      </c>
-      <c r="AU2" t="s" s="8">
-        <v>66</v>
-      </c>
-      <c r="AV2" t="s" s="8">
-        <v>86</v>
-      </c>
-      <c r="AW2" t="s" s="8">
-        <v>66</v>
-      </c>
-      <c r="AX2" t="s" s="8">
-        <v>87</v>
-      </c>
-      <c r="AY2" t="s" s="8">
-        <v>88</v>
-      </c>
-      <c r="AZ2" t="s" s="6">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="qa1@gogotech.hk "/>
-  </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
adding the optional remarks in delivery page
add the merchant remarks while fixing the transport landing page issue
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -175,7 +175,108 @@
     <t>DRIVER_PASSWORD</t>
   </si>
   <si>
-    <t>TC001_Complete a delivery order with testing business account</t>
+    <t>TC001_Complete a transport order with testing personal account</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="&quot;Helvetica Neue&quot;"/>
+      </rPr>
+      <t>qa1@gogotech.hk</t>
+    </r>
+  </si>
+  <si>
+    <t>Tin Hau</t>
+  </si>
+  <si>
+    <t>Tsim Sha Tsui</t>
+  </si>
+  <si>
+    <t>Chai wan</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>ASAP</t>
+  </si>
+  <si>
+    <t>No hourly rental</t>
+  </si>
+  <si>
+    <t>Van</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Tai Lam Tunnel</t>
+  </si>
+  <si>
+    <t>William Koh</t>
+  </si>
+  <si>
+    <t>No tip</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>North Point</t>
+  </si>
+  <si>
+    <t>3026A</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Siu Sai Wan</t>
+  </si>
+  <si>
+    <t>4218B</t>
+  </si>
+  <si>
+    <t>William2</t>
+  </si>
+  <si>
+    <t>Instant</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Testing delivery notes</t>
+  </si>
+  <si>
+    <t>Testing merchant order remarks</t>
+  </si>
+  <si>
+    <t>Aa123456</t>
+  </si>
+  <si>
+    <t>TC002_Cancel a transport order with testing personal account</t>
+  </si>
+  <si>
+    <t>Cityu</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Lion Rock Tunnel</t>
+  </si>
+  <si>
+    <t>TC003_Complete a transport order with testing business account</t>
   </si>
   <si>
     <t>Business</t>
@@ -184,73 +285,25 @@
     <t>qadmaster1@gogotech.hk</t>
   </si>
   <si>
-    <t>Tin Hau</t>
-  </si>
-  <si>
-    <t>Tsim Sha Tsui</t>
-  </si>
-  <si>
-    <t>Chai wan</t>
-  </si>
-  <si>
-    <t>Today</t>
-  </si>
-  <si>
-    <t>ASAP</t>
-  </si>
-  <si>
-    <t>No hourly rental</t>
-  </si>
-  <si>
-    <t>Van</t>
-  </si>
-  <si>
-    <t>Basic</t>
-  </si>
-  <si>
-    <t>Tai Lam Tunnel</t>
-  </si>
-  <si>
-    <t>William Koh</t>
-  </si>
-  <si>
-    <t>CASH</t>
+    <t>QA Tester</t>
+  </si>
+  <si>
+    <t>TC004_Cancel a transport order with testing business account</t>
+  </si>
+  <si>
+    <t>TC005_Complete a delivery order with testing personal account</t>
   </si>
   <si>
     <t>D</t>
   </si>
   <si>
-    <t>North Point</t>
-  </si>
-  <si>
-    <t>3026A</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>Chai Wan</t>
-  </si>
-  <si>
-    <t>4218B</t>
-  </si>
-  <si>
-    <t>William2</t>
-  </si>
-  <si>
-    <t>Instant</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>Testing delivery notes</t>
-  </si>
-  <si>
-    <t>Testing merchant order remarks</t>
-  </si>
-  <si>
-    <t>Aa123456</t>
+    <t>TC006_Cancel a delivery order with testing personal account</t>
+  </si>
+  <si>
+    <t>TC007_Complete a delivery order with testing business account</t>
+  </si>
+  <si>
+    <t>TC008_Cancel a delivery order with testing business account</t>
   </si>
 </sst>
 </file>
@@ -260,7 +313,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -283,6 +336,18 @@
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="8"/>
+      <color indexed="11"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="8"/>
       <color indexed="8"/>
       <name val="&quot;Helvetica Neue&quot;"/>
@@ -336,7 +401,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -349,13 +414,16 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -377,6 +445,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1411,13 +1480,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BB2"/>
+  <dimension ref="A1:BB9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="54" width="12.6719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="39.8516" style="1" customWidth="1"/>
+    <col min="2" max="54" width="12.6719" style="1" customWidth="1"/>
     <col min="55" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1592,10 +1662,10 @@
       <c r="B2" t="s" s="3">
         <v>55</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="4">
         <v>56</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>12345678</v>
       </c>
       <c r="E2" t="s" s="3">
@@ -1604,10 +1674,10 @@
       <c r="F2" t="s" s="3">
         <v>58</v>
       </c>
-      <c r="G2" t="b" s="5">
-        <v>0</v>
-      </c>
-      <c r="H2" t="b" s="5">
+      <c r="G2" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b" s="6">
         <v>0</v>
       </c>
       <c r="I2" t="s" s="3">
@@ -1631,125 +1701,1279 @@
       <c r="O2" t="s" s="3">
         <v>64</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="6">
         <v>4</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="6">
         <v>2</v>
       </c>
-      <c r="R2" t="b" s="5">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b" s="5">
-        <v>1</v>
-      </c>
-      <c r="T2" t="b" s="5">
-        <v>0</v>
-      </c>
-      <c r="U2" t="b" s="5">
-        <v>0</v>
-      </c>
-      <c r="V2" t="b" s="5">
+      <c r="R2" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="T2" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="V2" t="b" s="6">
         <v>0</v>
       </c>
       <c r="W2" t="s" s="3">
         <v>65</v>
       </c>
-      <c r="X2" t="b" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="b" s="5">
+      <c r="X2" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="b" s="6">
         <v>0</v>
       </c>
       <c r="Z2" t="s" s="3">
         <v>66</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AA2" s="6">
         <v>51112222</v>
       </c>
-      <c r="AB2" t="b" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="5">
+      <c r="AB2" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="6">
         <v>852</v>
       </c>
-      <c r="AD2" s="5">
-        <v>20</v>
-      </c>
-      <c r="AE2" t="b" s="5">
+      <c r="AD2" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="AE2" t="b" s="6">
         <v>0</v>
       </c>
       <c r="AF2" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="AG2" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="s" s="7">
+        <v>69</v>
+      </c>
+      <c r="AI2" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="AJ2" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="AK2" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>92516783</v>
+      </c>
+      <c r="AM2" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="AN2" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="AO2" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="AP2" s="5">
+        <v>53326890</v>
+      </c>
+      <c r="AQ2" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="AR2" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="AS2" s="5">
+        <v>30</v>
+      </c>
+      <c r="AT2" s="5">
+        <v>15</v>
+      </c>
+      <c r="AU2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AW2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="AY2" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="BA2" s="5">
+        <v>66778899</v>
+      </c>
+      <c r="BB2" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" ht="14" customHeight="1">
+      <c r="A3" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s" s="4">
+        <v>56</v>
+      </c>
+      <c r="D3" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E3" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="G3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J3" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="K3" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="M3" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="N3" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="O3" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="P3" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>1</v>
+      </c>
+      <c r="R3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="V3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="X3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>51112222</v>
+      </c>
+      <c r="AB3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>852</v>
+      </c>
+      <c r="AD3" t="s" s="3">
         <v>67</v>
       </c>
-      <c r="AG2" t="b" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH2" t="s" s="6">
+      <c r="AE3" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="s" s="3">
         <v>68</v>
       </c>
-      <c r="AI2" t="s" s="6">
+      <c r="AG3" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="s" s="7">
         <v>69</v>
       </c>
-      <c r="AJ2" t="s" s="6">
+      <c r="AI3" t="s" s="7">
         <v>70</v>
       </c>
-      <c r="AK2" t="s" s="6">
+      <c r="AJ3" t="s" s="7">
         <v>71</v>
       </c>
-      <c r="AL2" s="4">
+      <c r="AK3" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="AL3" s="5">
         <v>92516783</v>
       </c>
-      <c r="AM2" t="s" s="6">
+      <c r="AM3" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="AN3" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="AO3" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>53326890</v>
+      </c>
+      <c r="AQ3" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="AR3" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>30</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>15</v>
+      </c>
+      <c r="AU3" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AW3" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="AY3" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="BA3" s="5">
+        <v>66778899</v>
+      </c>
+      <c r="BB3" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" ht="14" customHeight="1">
+      <c r="A4" t="s" s="3">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s" s="3">
+        <v>87</v>
+      </c>
+      <c r="D4" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E4" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="G4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="K4" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="N4" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="O4" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="P4" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="U4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="V4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="X4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>51112222</v>
+      </c>
+      <c r="AB4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>852</v>
+      </c>
+      <c r="AD4" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="AE4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="AG4" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="s" s="7">
+        <v>69</v>
+      </c>
+      <c r="AI4" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="AJ4" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="AK4" t="s" s="7">
         <v>72</v>
       </c>
-      <c r="AN2" t="s" s="6">
+      <c r="AL4" s="5">
+        <v>92516783</v>
+      </c>
+      <c r="AM4" t="s" s="7">
         <v>73</v>
       </c>
-      <c r="AO2" t="s" s="6">
+      <c r="AN4" t="s" s="7">
         <v>74</v>
       </c>
-      <c r="AP2" s="4">
+      <c r="AO4" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="AP4" s="5">
         <v>53326890</v>
       </c>
-      <c r="AQ2" t="s" s="6">
+      <c r="AQ4" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="AR4" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="AS4" s="5">
+        <v>30</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>15</v>
+      </c>
+      <c r="AU4" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AW4" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX4" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="AY4" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ4" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="BA4" s="5">
+        <v>66778899</v>
+      </c>
+      <c r="BB4" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" ht="14" customHeight="1">
+      <c r="A5" t="s" s="3">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s" s="3">
+        <v>87</v>
+      </c>
+      <c r="D5" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E5" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="G5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J5" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="K5" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="L5" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="N5" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="O5" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="P5" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>1</v>
+      </c>
+      <c r="R5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="S5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="T5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="U5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="V5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="X5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>51112222</v>
+      </c>
+      <c r="AB5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="6">
+        <v>852</v>
+      </c>
+      <c r="AD5" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="AE5" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="AG5" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH5" t="s" s="7">
+        <v>69</v>
+      </c>
+      <c r="AI5" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="AJ5" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="AK5" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="AL5" s="5">
+        <v>92516783</v>
+      </c>
+      <c r="AM5" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="AN5" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="AO5" t="s" s="7">
         <v>75</v>
       </c>
-      <c r="AR2" t="s" s="6">
+      <c r="AP5" s="5">
+        <v>53326890</v>
+      </c>
+      <c r="AQ5" t="s" s="7">
         <v>76</v>
       </c>
-      <c r="AS2" s="4">
+      <c r="AR5" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="AS5" s="5">
         <v>30</v>
       </c>
-      <c r="AT2" s="4">
+      <c r="AT5" s="5">
         <v>15</v>
       </c>
-      <c r="AU2" t="b" s="4">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="4">
+      <c r="AU5" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="5">
         <v>1000</v>
       </c>
-      <c r="AW2" t="b" s="4">
-        <v>0</v>
-      </c>
-      <c r="AX2" t="s" s="6">
+      <c r="AW5" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX5" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="AY5" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ5" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>66778899</v>
+      </c>
+      <c r="BB5" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" ht="14" customHeight="1">
+      <c r="A6" t="s" s="3">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="G6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="J6" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="K6" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="L6" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="M6" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="N6" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="O6" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="P6" s="6">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>2</v>
+      </c>
+      <c r="R6" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="T6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="U6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="V6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="X6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>51112222</v>
+      </c>
+      <c r="AB6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="6">
+        <v>852</v>
+      </c>
+      <c r="AD6" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="AE6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="AG6" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="s" s="7">
+        <v>91</v>
+      </c>
+      <c r="AI6" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="AJ6" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="AK6" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="AL6" s="5">
+        <v>92516783</v>
+      </c>
+      <c r="AM6" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="AN6" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="AO6" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="AP6" s="5">
+        <v>53326890</v>
+      </c>
+      <c r="AQ6" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="AR6" t="s" s="7">
         <v>77</v>
       </c>
-      <c r="AY2" t="b" s="4">
+      <c r="AS6" s="5">
+        <v>30</v>
+      </c>
+      <c r="AT6" s="5">
+        <v>15</v>
+      </c>
+      <c r="AU6" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AW6" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX6" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="AY6" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ6" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="BA6" s="5">
+        <v>66778899</v>
+      </c>
+      <c r="BB6" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" ht="14" customHeight="1">
+      <c r="A7" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E7" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="G7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J7" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="K7" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="L7" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="N7" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="O7" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="P7" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="6">
         <v>1</v>
       </c>
-      <c r="AZ2" t="s" s="6">
+      <c r="R7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="S7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="T7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="U7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="V7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="W7" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="X7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>51112222</v>
+      </c>
+      <c r="AB7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>852</v>
+      </c>
+      <c r="AD7" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="AE7" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="AG7" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH7" t="s" s="7">
+        <v>91</v>
+      </c>
+      <c r="AI7" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="AJ7" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="AK7" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="AL7" s="5">
+        <v>92516783</v>
+      </c>
+      <c r="AM7" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="AN7" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="AO7" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="AP7" s="5">
+        <v>53326890</v>
+      </c>
+      <c r="AQ7" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="AR7" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="AS7" s="5">
+        <v>30</v>
+      </c>
+      <c r="AT7" s="5">
+        <v>15</v>
+      </c>
+      <c r="AU7" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AW7" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX7" t="s" s="7">
         <v>78</v>
       </c>
-      <c r="BA2" s="4">
+      <c r="AY7" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ7" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="BA7" s="5">
         <v>66778899</v>
       </c>
-      <c r="BB2" t="s" s="3">
+      <c r="BB7" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" ht="14" customHeight="1">
+      <c r="A8" t="s" s="3">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s" s="3">
+        <v>87</v>
+      </c>
+      <c r="D8" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E8" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="F8" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="G8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="K8" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="L8" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="N8" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="O8" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="P8" s="6">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>2</v>
+      </c>
+      <c r="R8" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="S8" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="T8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="U8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="V8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="W8" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="X8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>51112222</v>
+      </c>
+      <c r="AB8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="6">
+        <v>852</v>
+      </c>
+      <c r="AD8" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="AE8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="AG8" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="s" s="7">
+        <v>91</v>
+      </c>
+      <c r="AI8" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="AJ8" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="AK8" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="AL8" s="5">
+        <v>92516783</v>
+      </c>
+      <c r="AM8" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="AN8" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="AO8" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="AP8" s="5">
+        <v>53326890</v>
+      </c>
+      <c r="AQ8" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="AR8" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="AS8" s="5">
+        <v>30</v>
+      </c>
+      <c r="AT8" s="5">
+        <v>15</v>
+      </c>
+      <c r="AU8" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AW8" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX8" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="AY8" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ8" t="s" s="7">
         <v>79</v>
+      </c>
+      <c r="BA8" s="5">
+        <v>66778899</v>
+      </c>
+      <c r="BB8" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" ht="14" customHeight="1">
+      <c r="A9" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s" s="3">
+        <v>87</v>
+      </c>
+      <c r="D9" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E9" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="G9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="J9" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="K9" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="L9" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="M9" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="N9" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="O9" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="P9" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>1</v>
+      </c>
+      <c r="R9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="S9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="T9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="U9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="V9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="X9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>51112222</v>
+      </c>
+      <c r="AB9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>852</v>
+      </c>
+      <c r="AD9" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="AE9" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="AG9" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH9" t="s" s="7">
+        <v>91</v>
+      </c>
+      <c r="AI9" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="AJ9" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="AK9" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="AL9" s="5">
+        <v>92516783</v>
+      </c>
+      <c r="AM9" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="AN9" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="AO9" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="AP9" s="5">
+        <v>53326890</v>
+      </c>
+      <c r="AQ9" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="AR9" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="AS9" s="5">
+        <v>30</v>
+      </c>
+      <c r="AT9" s="5">
+        <v>15</v>
+      </c>
+      <c r="AU9" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AW9" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX9" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="AY9" t="b" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ9" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="BA9" s="5">
+        <v>66778899</v>
+      </c>
+      <c r="BB9" t="s" s="3">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="qa1@gogotech.hk"/>
+    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="qa1@gogotech.hk"/>
+    <hyperlink ref="C6" r:id="rId3" location="" tooltip="" display="qa1@gogotech.hk"/>
+    <hyperlink ref="C7" r:id="rId4" location="" tooltip="" display="qa1@gogotech.hk"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>